<commit_message>
feat: - upload order tables
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/одежда_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/одежда_по каждому размеру.xlsx
@@ -125,19 +125,19 @@
     <t xml:space="preserve">здесь ничего заполнять не нужно,. После внесения всех остальных колонок проверьте правильность заполнения данной колонки</t>
   </si>
   <si>
-    <t xml:space="preserve">Укажите торговую марку или бренд. Если ничего нет т укажите "Без товарного знака"</t>
+    <t xml:space="preserve">Укажите торговую марку или бренд. Если ничего нет оставьте пустым</t>
   </si>
   <si>
     <t xml:space="preserve">не заполнять</t>
   </si>
   <si>
-    <t xml:space="preserve">Указывайте конкретный артикул вашего Изделия. Заполнять обязательно. Если артикула на изделии нет то укажите любой произвольный</t>
+    <t xml:space="preserve">Указывайте конкретный артикул вашего Изделия или оставьте пустым</t>
   </si>
   <si>
     <t xml:space="preserve">выберите ВИД Одежды из выпадающего списка или со второго листа (справочник)</t>
   </si>
   <si>
-    <t xml:space="preserve">укажите конкретный цвет (справочник).</t>
+    <t xml:space="preserve">укажите конкретный цвет (см. справочник).</t>
   </si>
   <si>
     <t xml:space="preserve">Укажите пол для изделия</t>
@@ -6222,11 +6222,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.33"/>
@@ -19497,7 +19497,7 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="O6:Q6"/>
   </mergeCells>
-  <dataValidations count="10">
+  <dataValidations count="11">
     <dataValidation allowBlank="true" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B7:B9 L7:L8 B10:B45" type="textLength">
       <formula1>129</formula1>
       <formula2>0</formula2>
@@ -19506,7 +19506,7 @@
       <formula1>1025</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6 G6:H6" type="textLength">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H6" type="textLength">
       <formula1>129</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -19538,6 +19538,10 @@
       <formula1>100</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6 G6" type="textLength">
+      <formula1>129</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -19560,7 +19564,7 @@
       <selection pane="topLeft" activeCell="H160" activeCellId="0" sqref="H160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -23039,7 +23043,7 @@
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.4"/>
@@ -23751,7 +23755,7 @@
       <selection pane="topLeft" activeCell="A751" activeCellId="0" sqref="A751"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="246.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="246.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
upd:  - table clothes edit
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/одежда_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/одежда_по каждому размеру.xlsx
@@ -1129,7 +1129,7 @@
     <t xml:space="preserve">КАЙМАНОВЫ ОСТРОВА</t>
   </si>
   <si>
-    <t xml:space="preserve">ШЕЙНЫЙ ПЛАТОК</t>
+    <t xml:space="preserve">ПЛАТОК ШЕЙНЫЙ</t>
   </si>
   <si>
     <t xml:space="preserve">ХАКИ</t>
@@ -6228,7 +6228,7 @@
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.33"/>
@@ -19562,11 +19562,11 @@
   </sheetPr>
   <dimension ref="A1:J246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E229" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I243" activeCellId="0" sqref="I243"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D88" activeCellId="0" sqref="D88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -23043,7 +23043,7 @@
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.4"/>
@@ -23755,7 +23755,7 @@
       <selection pane="topLeft" activeCell="A751" activeCellId="0" sqref="A751"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="247.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="247.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
upd:  - clothes edit
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/одежда_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/одежда_по каждому размеру.xlsx
@@ -6228,7 +6228,7 @@
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.33"/>
@@ -19562,11 +19562,11 @@
   </sheetPr>
   <dimension ref="A1:J246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D88" activeCellId="0" sqref="D88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -19973,7 +19973,7 @@
         <v>142</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>143</v>
@@ -23043,7 +23043,7 @@
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.4"/>
@@ -23755,7 +23755,7 @@
       <selection pane="topLeft" activeCell="A751" activeCellId="0" sqref="A751"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="247.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="247.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>

</xml_diff>